<commit_message>
Updates on qualitative analysis spreadsheet
</commit_message>
<xml_diff>
--- a/data/experts/qualitative_analysis_data/third_round_chandler/Praveen.xlsx
+++ b/data/experts/qualitative_analysis_data/third_round_chandler/Praveen.xlsx
@@ -1,20 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fronchettl\Documents\GitHub\TOCHI-2023\data\experts\qualitative_analysis_data\third_round_chandler\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298A8628-7474-4AC7-822E-6927C347E73A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7913" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Raw" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Interview Analysis (Felipe)" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Interview Analysis (Haley)" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Interview Analysis (Chandler)" sheetId="4" r:id="rId7"/>
+    <sheet name="Raw" sheetId="1" r:id="rId1"/>
+    <sheet name="Interview Analysis (Felipe)" sheetId="2" r:id="rId2"/>
+    <sheet name="Interview Analysis (Haley)" sheetId="3" r:id="rId3"/>
+    <sheet name="Interview Analysis (Chandler)" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="41">
   <si>
     <t>Paragraphs</t>
   </si>
@@ -118,13 +127,7 @@
     <t>Participant: Enlarge the handles so that it can recognise mispinches</t>
   </si>
   <si>
-    <t>Easy to use and understand; Problem: Gripping/Pinching the interface can be difficult. Problem: There is a delay between the movement in mixed reality and the robot.</t>
-  </si>
-  <si>
     <t>Highlight : Bounding box is easy to use and understand;</t>
-  </si>
-  <si>
-    <t>Easy to understand; Could be used for moving large boxes in a warehouse;  Application: The interface could be used for distant manipulation.</t>
   </si>
   <si>
     <t xml:space="preserve">Application: Could be used for moving large boxes in a warehouse; </t>
@@ -144,48 +147,51 @@
   <si>
     <t>Suggestion: Move the controls for up and down movement;</t>
   </si>
-  <si>
-    <t xml:space="preserve">Suggestion: instructions to highlight capabilties; Snap position and coirdinate system; Fix the delay between interaction and movement of the robot; Improve grabbing recongnition; Move the controls for up and down movement; </t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -199,85 +205,87 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CC"/>
-        <bgColor rgb="FFFFF2CC"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
     <dxf>
-      <font/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
-      <border/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -467,24 +475,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Y33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="67.88"/>
-    <col customWidth="1" min="2" max="2" width="56.88"/>
+    <col min="1" max="1" width="67.86328125" customWidth="1"/>
+    <col min="2" max="2" width="56.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="26.25" customHeight="1">
+    <row r="1" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +526,7 @@
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -544,7 +555,7 @@
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -573,37 +584,37 @@
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -632,7 +643,7 @@
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
@@ -661,7 +672,7 @@
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
@@ -690,7 +701,7 @@
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -719,7 +730,7 @@
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
@@ -748,7 +759,7 @@
       <c r="X14" s="3"/>
       <c r="Y14" s="3"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -777,12 +788,12 @@
       <c r="X15" s="3"/>
       <c r="Y15" s="3"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
@@ -811,7 +822,7 @@
       <c r="X17" s="3"/>
       <c r="Y17" s="3"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
@@ -840,7 +851,7 @@
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
@@ -869,27 +880,27 @@
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>24</v>
       </c>
@@ -918,7 +929,7 @@
       <c r="X24" s="3"/>
       <c r="Y24" s="3"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
@@ -947,7 +958,7 @@
       <c r="X25" s="3"/>
       <c r="Y25" s="3"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
         <v>26</v>
       </c>
@@ -976,7 +987,7 @@
       <c r="X26" s="3"/>
       <c r="Y26" s="3"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
         <v>27</v>
       </c>
@@ -1005,7 +1016,7 @@
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
         <v>28</v>
       </c>
@@ -1034,57 +1045,58 @@
       <c r="X28" s="3"/>
       <c r="Y28" s="3"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A30" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A33">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Participant">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Participant">
       <formula>NOT(ISERROR(SEARCH(("Participant"),(A1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF3C78D8"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Y110"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="67.88"/>
-    <col customWidth="1" min="2" max="2" width="56.88"/>
+    <col min="1" max="1" width="67.86328125" customWidth="1"/>
+    <col min="2" max="2" width="56.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="26.25" customHeight="1">
+    <row r="1" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1115,7 +1127,7 @@
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
     </row>
-    <row r="2" ht="107.25" customHeight="1">
+    <row r="2" spans="1:25" ht="107.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1144,7 +1156,7 @@
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1173,7 +1185,7 @@
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1202,7 +1214,7 @@
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -1231,7 +1243,7 @@
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -1260,62 +1272,62 @@
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
@@ -1344,7 +1356,7 @@
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
@@ -1373,7 +1385,7 @@
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
@@ -1402,7 +1414,7 @@
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
@@ -1431,7 +1443,7 @@
       <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
@@ -1460,7 +1472,7 @@
       <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
@@ -1489,12 +1501,12 @@
       <c r="X23" s="3"/>
       <c r="Y23" s="3"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
@@ -1523,7 +1535,7 @@
       <c r="X25" s="3"/>
       <c r="Y25" s="3"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
         <v>26</v>
       </c>
@@ -1552,7 +1564,7 @@
       <c r="X26" s="3"/>
       <c r="Y26" s="3"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
         <v>27</v>
       </c>
@@ -1581,12 +1593,12 @@
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
         <v>29</v>
       </c>
@@ -1615,7 +1627,7 @@
       <c r="X29" s="3"/>
       <c r="Y29" s="3"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A30" s="4" t="s">
         <v>30</v>
       </c>
@@ -1644,17 +1656,17 @@
       <c r="X30" s="3"/>
       <c r="Y30" s="3"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
         <v>33</v>
       </c>
@@ -1683,12 +1695,12 @@
       <c r="X33" s="3"/>
       <c r="Y33" s="3"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:25" ht="15" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A35" s="4" t="s">
         <v>2</v>
       </c>
@@ -1717,7 +1729,7 @@
       <c r="X35" s="3"/>
       <c r="Y35" s="3"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A36" s="4" t="s">
         <v>3</v>
       </c>
@@ -1746,7 +1758,7 @@
       <c r="X36" s="3"/>
       <c r="Y36" s="3"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A37" s="4" t="s">
         <v>4</v>
       </c>
@@ -1775,52 +1787,52 @@
       <c r="X37" s="3"/>
       <c r="Y37" s="3"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A38" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A39" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A40" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A41" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A42" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A43" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A44" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A45" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A46" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A47" s="4" t="s">
         <v>14</v>
       </c>
@@ -1849,7 +1861,7 @@
       <c r="X47" s="3"/>
       <c r="Y47" s="3"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
         <v>15</v>
       </c>
@@ -1878,7 +1890,7 @@
       <c r="X48" s="3"/>
       <c r="Y48" s="3"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A49" s="4" t="s">
         <v>16</v>
       </c>
@@ -1907,7 +1919,7 @@
       <c r="X49" s="3"/>
       <c r="Y49" s="3"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A50" s="4" t="s">
         <v>17</v>
       </c>
@@ -1936,7 +1948,7 @@
       <c r="X50" s="3"/>
       <c r="Y50" s="3"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A51" s="4" t="s">
         <v>18</v>
       </c>
@@ -1965,7 +1977,7 @@
       <c r="X51" s="3"/>
       <c r="Y51" s="3"/>
     </row>
-    <row r="52">
+    <row r="52" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A52" s="4" t="s">
         <v>19</v>
       </c>
@@ -1994,7 +2006,7 @@
       <c r="X52" s="3"/>
       <c r="Y52" s="3"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A53" s="4" t="s">
         <v>20</v>
       </c>
@@ -2023,7 +2035,7 @@
       <c r="X53" s="3"/>
       <c r="Y53" s="3"/>
     </row>
-    <row r="54">
+    <row r="54" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A54" s="4" t="s">
         <v>21</v>
       </c>
@@ -2052,7 +2064,7 @@
       <c r="X54" s="3"/>
       <c r="Y54" s="3"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A55" s="4" t="s">
         <v>22</v>
       </c>
@@ -2081,7 +2093,7 @@
       <c r="X55" s="3"/>
       <c r="Y55" s="3"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A56" s="4" t="s">
         <v>23</v>
       </c>
@@ -2110,280 +2122,281 @@
       <c r="X56" s="3"/>
       <c r="Y56" s="3"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A57" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A58" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A59" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A60" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A61" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A62" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A63" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A64" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A65" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A66" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:1" ht="15" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A68" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A69" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A70" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A71" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A72" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A73" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A74" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:1" ht="45" x14ac:dyDescent="0.4">
       <c r="A75" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A76" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A77" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A78" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A79" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:1" ht="45" x14ac:dyDescent="0.4">
       <c r="A80" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:1" ht="45" x14ac:dyDescent="0.4">
       <c r="A81" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A82" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A83" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A84" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A85" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:1" ht="45" x14ac:dyDescent="0.4">
       <c r="A86" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A87" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:1" ht="45" x14ac:dyDescent="0.4">
       <c r="A88" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A89" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:1" ht="45" x14ac:dyDescent="0.4">
       <c r="A90" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A91" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A92" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A93" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A94" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A95" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A96" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A97" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A98" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A99" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A100" s="4"/>
     </row>
-    <row r="101">
+    <row r="101" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A101" s="4"/>
     </row>
-    <row r="102">
+    <row r="102" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A102" s="4"/>
     </row>
-    <row r="103">
+    <row r="103" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A103" s="4"/>
     </row>
-    <row r="104">
+    <row r="104" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A104" s="4"/>
     </row>
-    <row r="105">
+    <row r="105" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A105" s="4"/>
     </row>
-    <row r="106">
+    <row r="106" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A106" s="4"/>
     </row>
-    <row r="107">
+    <row r="107" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A107" s="4"/>
     </row>
-    <row r="108">
+    <row r="108" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A108" s="4"/>
     </row>
-    <row r="109">
+    <row r="109" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A109" s="4"/>
     </row>
-    <row r="110">
+    <row r="110" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A110" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A99">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Participant">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Participant">
       <formula>NOT(ISERROR(SEARCH(("Participant"),(A1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFF1C232"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Y110"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="67.88"/>
-    <col customWidth="1" min="2" max="2" width="56.88"/>
+    <col min="1" max="1" width="67.86328125" customWidth="1"/>
+    <col min="2" max="2" width="56.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="26.25" customHeight="1">
+    <row r="1" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2414,7 +2427,7 @@
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
     </row>
-    <row r="2" ht="107.25" customHeight="1">
+    <row r="2" spans="1:25" ht="107.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -2443,7 +2456,7 @@
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -2472,7 +2485,7 @@
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -2501,7 +2514,7 @@
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -2530,7 +2543,7 @@
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -2559,62 +2572,62 @@
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
@@ -2643,7 +2656,7 @@
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
@@ -2672,7 +2685,7 @@
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
@@ -2701,7 +2714,7 @@
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
@@ -2730,7 +2743,7 @@
       <c r="X21" s="3"/>
       <c r="Y21" s="3"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
@@ -2759,7 +2772,7 @@
       <c r="X22" s="3"/>
       <c r="Y22" s="3"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
@@ -2788,12 +2801,12 @@
       <c r="X23" s="3"/>
       <c r="Y23" s="3"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
@@ -2822,7 +2835,7 @@
       <c r="X25" s="3"/>
       <c r="Y25" s="3"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
         <v>26</v>
       </c>
@@ -2851,7 +2864,7 @@
       <c r="X26" s="3"/>
       <c r="Y26" s="3"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
         <v>27</v>
       </c>
@@ -2880,12 +2893,12 @@
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
         <v>29</v>
       </c>
@@ -2914,7 +2927,7 @@
       <c r="X29" s="3"/>
       <c r="Y29" s="3"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A30" s="4" t="s">
         <v>30</v>
       </c>
@@ -2943,17 +2956,17 @@
       <c r="X30" s="3"/>
       <c r="Y30" s="3"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
         <v>33</v>
       </c>
@@ -2982,12 +2995,12 @@
       <c r="X33" s="3"/>
       <c r="Y33" s="3"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:25" ht="15" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A35" s="4" t="s">
         <v>2</v>
       </c>
@@ -3016,7 +3029,7 @@
       <c r="X35" s="3"/>
       <c r="Y35" s="3"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A36" s="4" t="s">
         <v>3</v>
       </c>
@@ -3045,7 +3058,7 @@
       <c r="X36" s="3"/>
       <c r="Y36" s="3"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A37" s="4" t="s">
         <v>4</v>
       </c>
@@ -3074,52 +3087,52 @@
       <c r="X37" s="3"/>
       <c r="Y37" s="3"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A38" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A39" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A40" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A41" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A42" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A43" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A44" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A45" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A46" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A47" s="4" t="s">
         <v>14</v>
       </c>
@@ -3148,7 +3161,7 @@
       <c r="X47" s="3"/>
       <c r="Y47" s="3"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
         <v>15</v>
       </c>
@@ -3177,7 +3190,7 @@
       <c r="X48" s="3"/>
       <c r="Y48" s="3"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A49" s="4" t="s">
         <v>16</v>
       </c>
@@ -3206,7 +3219,7 @@
       <c r="X49" s="3"/>
       <c r="Y49" s="3"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A50" s="4" t="s">
         <v>17</v>
       </c>
@@ -3235,7 +3248,7 @@
       <c r="X50" s="3"/>
       <c r="Y50" s="3"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A51" s="4" t="s">
         <v>18</v>
       </c>
@@ -3264,7 +3277,7 @@
       <c r="X51" s="3"/>
       <c r="Y51" s="3"/>
     </row>
-    <row r="52">
+    <row r="52" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A52" s="4" t="s">
         <v>19</v>
       </c>
@@ -3293,7 +3306,7 @@
       <c r="X52" s="3"/>
       <c r="Y52" s="3"/>
     </row>
-    <row r="53">
+    <row r="53" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A53" s="4" t="s">
         <v>20</v>
       </c>
@@ -3322,7 +3335,7 @@
       <c r="X53" s="3"/>
       <c r="Y53" s="3"/>
     </row>
-    <row r="54">
+    <row r="54" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A54" s="4" t="s">
         <v>21</v>
       </c>
@@ -3351,7 +3364,7 @@
       <c r="X54" s="3"/>
       <c r="Y54" s="3"/>
     </row>
-    <row r="55">
+    <row r="55" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A55" s="4" t="s">
         <v>22</v>
       </c>
@@ -3380,7 +3393,7 @@
       <c r="X55" s="3"/>
       <c r="Y55" s="3"/>
     </row>
-    <row r="56">
+    <row r="56" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A56" s="4" t="s">
         <v>23</v>
       </c>
@@ -3409,280 +3422,283 @@
       <c r="X56" s="3"/>
       <c r="Y56" s="3"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:25" ht="45" x14ac:dyDescent="0.4">
       <c r="A57" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A58" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A59" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A60" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A61" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:25" ht="30" x14ac:dyDescent="0.4">
       <c r="A62" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A63" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:25" ht="15" x14ac:dyDescent="0.4">
       <c r="A64" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A65" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A66" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:1" ht="15" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A68" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A69" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A70" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A71" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A72" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A73" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A74" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:1" ht="45" x14ac:dyDescent="0.4">
       <c r="A75" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A76" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A77" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A78" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A79" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:1" ht="45" x14ac:dyDescent="0.4">
       <c r="A80" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:1" ht="45" x14ac:dyDescent="0.4">
       <c r="A81" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A82" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A83" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A84" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A85" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:1" ht="45" x14ac:dyDescent="0.4">
       <c r="A86" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A87" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:1" ht="45" x14ac:dyDescent="0.4">
       <c r="A88" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A89" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:1" ht="45" x14ac:dyDescent="0.4">
       <c r="A90" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A91" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A92" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A93" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A94" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:1" ht="30" x14ac:dyDescent="0.4">
       <c r="A95" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A96" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A97" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A98" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A99" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A100" s="4"/>
     </row>
-    <row r="101">
+    <row r="101" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A101" s="4"/>
     </row>
-    <row r="102">
+    <row r="102" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A102" s="4"/>
     </row>
-    <row r="103">
+    <row r="103" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A103" s="4"/>
     </row>
-    <row r="104">
+    <row r="104" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A104" s="4"/>
     </row>
-    <row r="105">
+    <row r="105" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A105" s="4"/>
     </row>
-    <row r="106">
+    <row r="106" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A106" s="4"/>
     </row>
-    <row r="107">
+    <row r="107" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A107" s="4"/>
     </row>
-    <row r="108">
+    <row r="108" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A108" s="4"/>
     </row>
-    <row r="109">
+    <row r="109" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A109" s="4"/>
     </row>
-    <row r="110">
+    <row r="110" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A110" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A99">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Participant">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Participant">
       <formula>NOT(ISERROR(SEARCH(("Participant"),(A1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF6AA84F"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:X110"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="67.88"/>
-    <col customWidth="1" min="2" max="2" width="56.88"/>
+    <col min="1" max="1" width="67.86328125" customWidth="1"/>
+    <col min="2" max="2" width="51.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="26.25" customHeight="1">
+    <row r="1" spans="1:24" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3711,9 +3727,8 @@
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-    </row>
-    <row r="2" ht="107.25" customHeight="1">
+    </row>
+    <row r="2" spans="1:24" ht="107.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -3740,15 +3755,12 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-    </row>
-    <row r="3">
+    </row>
+    <row r="3" spans="1:24" ht="30" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -3771,12 +3783,12 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-    </row>
-    <row r="4">
+    </row>
+    <row r="4" spans="1:24" ht="30" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -3799,12 +3811,12 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-    </row>
-    <row r="5">
+    </row>
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -3827,12 +3839,12 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-    </row>
-    <row r="6">
+    </row>
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -3855,101 +3867,90 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-    </row>
-    <row r="7">
+    </row>
+    <row r="7" spans="1:24" ht="30" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:24" ht="30" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:24" ht="45" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="B10" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="30" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:24" ht="30" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13">
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:24" ht="30" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14">
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:24" ht="45" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15">
+      <c r="B14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:24" ht="45" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J15" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16">
+      <c r="B15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17">
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:24" ht="30" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18">
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:24" ht="30" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="I18" s="6"/>
+      <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
@@ -3964,22 +3965,20 @@
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
-    </row>
-    <row r="19">
+    </row>
+    <row r="19" spans="1:24" ht="30" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
@@ -3994,12 +3993,12 @@
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
-    </row>
-    <row r="20">
+    </row>
+    <row r="20" spans="1:24" ht="45" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -4022,15 +4021,15 @@
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-    </row>
-    <row r="21">
+    </row>
+    <row r="21" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="B21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -4052,15 +4051,15 @@
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
-    </row>
-    <row r="22">
+    </row>
+    <row r="22" spans="1:24" ht="45" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>37</v>
-      </c>
+      <c r="B22" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -4082,9 +4081,8 @@
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
-      <c r="Y22" s="3"/>
-    </row>
-    <row r="23">
+    </row>
+    <row r="23" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
@@ -4111,19 +4109,21 @@
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
-    </row>
-    <row r="24">
+    </row>
+    <row r="24" spans="1:24" ht="45" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" ht="30" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
         <v>25</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -4147,12 +4147,12 @@
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
-      <c r="Y25" s="3"/>
-    </row>
-    <row r="26">
+    </row>
+    <row r="26" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -4175,11 +4175,13 @@
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
-      <c r="Y26" s="3"/>
-    </row>
-    <row r="27">
+    </row>
+    <row r="27" spans="1:24" ht="30" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
         <v>27</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -4203,17 +4205,20 @@
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
-      <c r="Y27" s="3"/>
-    </row>
-    <row r="28">
+    </row>
+    <row r="28" spans="1:24" ht="30" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="29">
+      <c r="B28" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" ht="30" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -4236,12 +4241,12 @@
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
-      <c r="Y29" s="3"/>
-    </row>
-    <row r="30">
+    </row>
+    <row r="30" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A30" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -4264,31 +4269,27 @@
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
-      <c r="Y30" s="3"/>
-    </row>
-    <row r="31">
+    </row>
+    <row r="31" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32">
+      <c r="B31" s="5"/>
+    </row>
+    <row r="32" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33">
+      <c r="B32" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -4310,20 +4311,15 @@
       <c r="V33" s="3"/>
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
-      <c r="Y33" s="3"/>
-    </row>
-    <row r="34">
+    </row>
+    <row r="34" spans="1:24" ht="15" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
-      <c r="C34" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35">
+      <c r="B34" s="5"/>
+    </row>
+    <row r="35" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A35" s="4"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -4345,9 +4341,8 @@
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
       <c r="X35" s="3"/>
-      <c r="Y35" s="3"/>
-    </row>
-    <row r="36">
+    </row>
+    <row r="36" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -4372,9 +4367,8 @@
       <c r="V36" s="3"/>
       <c r="W36" s="3"/>
       <c r="X36" s="3"/>
-      <c r="Y36" s="3"/>
-    </row>
-    <row r="37">
+    </row>
+    <row r="37" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -4399,44 +4393,35 @@
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
-      <c r="Y37" s="3"/>
-    </row>
-    <row r="38">
+    </row>
+    <row r="38" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A38" s="4"/>
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39">
+    </row>
+    <row r="39" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A39" s="4"/>
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40">
+    </row>
+    <row r="40" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A40" s="4"/>
-      <c r="B40" s="3"/>
-    </row>
-    <row r="41">
+    </row>
+    <row r="41" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A41" s="4"/>
-      <c r="B41" s="3"/>
-    </row>
-    <row r="42">
+    </row>
+    <row r="42" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A42" s="4"/>
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43">
+    </row>
+    <row r="43" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A43" s="4"/>
-      <c r="B43" s="3"/>
-    </row>
-    <row r="44">
+    </row>
+    <row r="44" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A44" s="4"/>
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45">
+    </row>
+    <row r="45" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A45" s="4"/>
-      <c r="B45" s="3"/>
-    </row>
-    <row r="46">
+    </row>
+    <row r="46" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A46" s="4"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A47" s="4"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -4461,9 +4446,8 @@
       <c r="V47" s="3"/>
       <c r="W47" s="3"/>
       <c r="X47" s="3"/>
-      <c r="Y47" s="3"/>
-    </row>
-    <row r="48">
+    </row>
+    <row r="48" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A48" s="4"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -4488,9 +4472,8 @@
       <c r="V48" s="3"/>
       <c r="W48" s="3"/>
       <c r="X48" s="3"/>
-      <c r="Y48" s="3"/>
-    </row>
-    <row r="49">
+    </row>
+    <row r="49" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A49" s="4"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -4515,9 +4498,8 @@
       <c r="V49" s="3"/>
       <c r="W49" s="3"/>
       <c r="X49" s="3"/>
-      <c r="Y49" s="3"/>
-    </row>
-    <row r="50">
+    </row>
+    <row r="50" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A50" s="4"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -4542,9 +4524,8 @@
       <c r="V50" s="3"/>
       <c r="W50" s="3"/>
       <c r="X50" s="3"/>
-      <c r="Y50" s="3"/>
-    </row>
-    <row r="51">
+    </row>
+    <row r="51" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A51" s="4"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -4569,9 +4550,8 @@
       <c r="V51" s="3"/>
       <c r="W51" s="3"/>
       <c r="X51" s="3"/>
-      <c r="Y51" s="3"/>
-    </row>
-    <row r="52">
+    </row>
+    <row r="52" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A52" s="4"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -4596,9 +4576,8 @@
       <c r="V52" s="3"/>
       <c r="W52" s="3"/>
       <c r="X52" s="3"/>
-      <c r="Y52" s="3"/>
-    </row>
-    <row r="53">
+    </row>
+    <row r="53" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A53" s="4"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -4623,9 +4602,8 @@
       <c r="V53" s="3"/>
       <c r="W53" s="3"/>
       <c r="X53" s="3"/>
-      <c r="Y53" s="3"/>
-    </row>
-    <row r="54">
+    </row>
+    <row r="54" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A54" s="4"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -4650,9 +4628,8 @@
       <c r="V54" s="3"/>
       <c r="W54" s="3"/>
       <c r="X54" s="3"/>
-      <c r="Y54" s="3"/>
-    </row>
-    <row r="55">
+    </row>
+    <row r="55" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A55" s="4"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -4677,9 +4654,8 @@
       <c r="V55" s="3"/>
       <c r="W55" s="3"/>
       <c r="X55" s="3"/>
-      <c r="Y55" s="3"/>
-    </row>
-    <row r="56">
+    </row>
+    <row r="56" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A56" s="4"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -4704,181 +4680,175 @@
       <c r="V56" s="3"/>
       <c r="W56" s="3"/>
       <c r="X56" s="3"/>
-      <c r="Y56" s="3"/>
-    </row>
-    <row r="57">
+    </row>
+    <row r="57" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A57" s="4"/>
     </row>
-    <row r="58">
+    <row r="58" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A58" s="4"/>
     </row>
-    <row r="59">
+    <row r="59" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A59" s="4"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A60" s="4"/>
     </row>
-    <row r="61">
+    <row r="61" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A61" s="4"/>
     </row>
-    <row r="62">
+    <row r="62" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A62" s="4"/>
     </row>
-    <row r="63">
+    <row r="63" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A63" s="4"/>
     </row>
-    <row r="64">
+    <row r="64" spans="1:24" ht="15" x14ac:dyDescent="0.4">
       <c r="A64" s="4"/>
     </row>
-    <row r="65">
+    <row r="65" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A65" s="4"/>
     </row>
-    <row r="66">
+    <row r="66" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A66" s="4"/>
     </row>
-    <row r="67">
+    <row r="67" spans="1:1" ht="15" x14ac:dyDescent="0.35">
       <c r="A67" s="1"/>
     </row>
-    <row r="68">
+    <row r="68" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A68" s="4"/>
     </row>
-    <row r="69">
+    <row r="69" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A69" s="4"/>
     </row>
-    <row r="70">
+    <row r="70" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A70" s="4"/>
     </row>
-    <row r="71">
+    <row r="71" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A71" s="4"/>
     </row>
-    <row r="72">
+    <row r="72" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A72" s="4"/>
     </row>
-    <row r="73">
+    <row r="73" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A73" s="4"/>
     </row>
-    <row r="74">
+    <row r="74" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A74" s="4"/>
     </row>
-    <row r="75">
+    <row r="75" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A75" s="4"/>
     </row>
-    <row r="76">
+    <row r="76" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A76" s="4"/>
     </row>
-    <row r="77">
+    <row r="77" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A77" s="4"/>
     </row>
-    <row r="78">
+    <row r="78" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A78" s="4"/>
     </row>
-    <row r="79">
+    <row r="79" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A79" s="4"/>
     </row>
-    <row r="80">
+    <row r="80" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A80" s="4"/>
     </row>
-    <row r="81">
+    <row r="81" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A81" s="4"/>
     </row>
-    <row r="82">
+    <row r="82" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A82" s="4"/>
     </row>
-    <row r="83">
+    <row r="83" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A83" s="4"/>
     </row>
-    <row r="84">
+    <row r="84" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A84" s="4"/>
     </row>
-    <row r="85">
+    <row r="85" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A85" s="4"/>
     </row>
-    <row r="86">
+    <row r="86" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A86" s="4"/>
     </row>
-    <row r="87">
+    <row r="87" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A87" s="4"/>
     </row>
-    <row r="88">
+    <row r="88" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A88" s="4"/>
     </row>
-    <row r="89">
+    <row r="89" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A89" s="4"/>
     </row>
-    <row r="90">
+    <row r="90" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A90" s="4"/>
     </row>
-    <row r="91">
+    <row r="91" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A91" s="4"/>
     </row>
-    <row r="92">
+    <row r="92" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A92" s="4"/>
     </row>
-    <row r="93">
+    <row r="93" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A93" s="4"/>
     </row>
-    <row r="94">
+    <row r="94" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A94" s="4"/>
     </row>
-    <row r="95">
+    <row r="95" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A95" s="4"/>
     </row>
-    <row r="96">
+    <row r="96" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A96" s="4"/>
     </row>
-    <row r="97">
+    <row r="97" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A97" s="4"/>
     </row>
-    <row r="98">
+    <row r="98" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A98" s="4"/>
     </row>
-    <row r="99">
+    <row r="99" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A99" s="4"/>
     </row>
-    <row r="100">
+    <row r="100" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A100" s="4"/>
     </row>
-    <row r="101">
+    <row r="101" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A101" s="4"/>
     </row>
-    <row r="102">
+    <row r="102" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A102" s="4"/>
     </row>
-    <row r="103">
+    <row r="103" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A103" s="4"/>
     </row>
-    <row r="104">
+    <row r="104" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A104" s="4"/>
     </row>
-    <row r="105">
+    <row r="105" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A105" s="4"/>
     </row>
-    <row r="106">
+    <row r="106" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A106" s="4"/>
     </row>
-    <row r="107">
+    <row r="107" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A107" s="4"/>
     </row>
-    <row r="108">
+    <row r="108" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A108" s="4"/>
     </row>
-    <row r="109">
+    <row r="109" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A109" s="4"/>
     </row>
-    <row r="110">
+    <row r="110" spans="1:1" ht="15" x14ac:dyDescent="0.4">
       <c r="A110" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B3:B12"/>
-    <mergeCell ref="B14:B22"/>
-    <mergeCell ref="B24:B33"/>
-  </mergeCells>
   <conditionalFormatting sqref="A1:A99">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Participant">
       <formula>NOT(ISERROR(SEARCH(("Participant"),(A1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>